<commit_message>
cleaning prior to sharing
</commit_message>
<xml_diff>
--- a/data/Database_IPGP.xlsx
+++ b/data/Database_IPGP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VISCO" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5379" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5379" uniqueCount="444">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -837,9 +837,6 @@
     <t xml:space="preserve">MM1932</t>
   </si>
   <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
     <t xml:space="preserve">FP1938</t>
   </si>
   <si>
@@ -1532,7 +1529,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1621,16 +1618,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1749,7 +1742,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2019,11 +2012,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="14695490"/>
-        <c:axId val="23347743"/>
+        <c:axId val="82597131"/>
+        <c:axId val="59730243"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14695490"/>
+        <c:axId val="82597131"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2055,12 +2048,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23347743"/>
+        <c:crossAx val="59730243"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23347743"/>
+        <c:axId val="59730243"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2102,7 +2095,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14695490"/>
+        <c:crossAx val="82597131"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2153,7 +2146,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2266,11 +2259,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="35273775"/>
-        <c:axId val="92784825"/>
+        <c:axId val="92538547"/>
+        <c:axId val="29422682"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="35273775"/>
+        <c:axId val="92538547"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2298,12 +2291,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92784825"/>
+        <c:crossAx val="29422682"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92784825"/>
+        <c:axId val="29422682"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2340,7 +2333,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35273775"/>
+        <c:crossAx val="92538547"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2388,7 +2381,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2957,11 +2950,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="70072064"/>
-        <c:axId val="46131792"/>
+        <c:axId val="29260820"/>
+        <c:axId val="34125466"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70072064"/>
+        <c:axId val="29260820"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,12 +2982,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46131792"/>
+        <c:crossAx val="34125466"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46131792"/>
+        <c:axId val="34125466"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3031,7 +3024,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70072064"/>
+        <c:crossAx val="29260820"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3090,9 +3083,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>127080</xdr:colOff>
+      <xdr:colOff>126720</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>214920</xdr:rowOff>
+      <xdr:rowOff>214560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3101,7 +3094,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2639880" y="6742080"/>
-        <a:ext cx="4576680" cy="3353400"/>
+        <a:ext cx="4576320" cy="3353040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3120,9 +3113,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>266400</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3131,7 +3124,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6357240" y="4240800"/>
-        <a:ext cx="5758560" cy="3238560"/>
+        <a:ext cx="5758200" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3150,9 +3143,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>297720</xdr:colOff>
+      <xdr:colOff>297360</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3161,7 +3154,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8961840" y="16893000"/>
-        <a:ext cx="5762880" cy="3249000"/>
+        <a:ext cx="5762520" cy="3248640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3181,7 +3174,7 @@
   </sheetPr>
   <dimension ref="A1:AB1961"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1005" topLeftCell="L1951" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="F1951" activeCellId="0" sqref="F1951"/>
@@ -67604,10 +67597,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ341"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A341" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="795" topLeftCell="A1" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A341" activeCellId="0" sqref="A341"/>
-      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="795" topLeftCell="A286" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="L298" activeCellId="0" sqref="L298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -68994,7 +68987,7 @@
       <c r="G53" s="23" t="n">
         <v>1.52034</v>
       </c>
-      <c r="H53" s="24" t="s">
+      <c r="H53" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69020,7 +69013,7 @@
       <c r="G54" s="23" t="n">
         <v>1.51496</v>
       </c>
-      <c r="H54" s="24" t="s">
+      <c r="H54" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69046,7 +69039,7 @@
       <c r="G55" s="23" t="n">
         <v>1.51361</v>
       </c>
-      <c r="H55" s="24" t="s">
+      <c r="H55" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69072,7 +69065,7 @@
       <c r="G56" s="23" t="n">
         <v>1.5097</v>
       </c>
-      <c r="H56" s="24" t="s">
+      <c r="H56" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69098,7 +69091,7 @@
       <c r="G57" s="23" t="n">
         <v>1.50865</v>
       </c>
-      <c r="H57" s="24" t="s">
+      <c r="H57" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69124,7 +69117,7 @@
       <c r="G58" s="23" t="n">
         <v>1.50023</v>
       </c>
-      <c r="H58" s="24" t="s">
+      <c r="H58" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69150,7 +69143,7 @@
       <c r="G59" s="23" t="n">
         <v>1.49615</v>
       </c>
-      <c r="H59" s="24" t="s">
+      <c r="H59" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69176,7 +69169,7 @@
       <c r="G60" s="23" t="n">
         <v>1.49425</v>
       </c>
-      <c r="H60" s="24" t="s">
+      <c r="H60" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69202,7 +69195,7 @@
       <c r="G61" s="23" t="n">
         <v>1.49121</v>
       </c>
-      <c r="H61" s="24" t="s">
+      <c r="H61" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69228,7 +69221,7 @@
       <c r="G62" s="23" t="n">
         <v>1.48892</v>
       </c>
-      <c r="H62" s="24" t="s">
+      <c r="H62" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69254,7 +69247,7 @@
       <c r="G63" s="23" t="n">
         <v>1.48738</v>
       </c>
-      <c r="H63" s="24" t="s">
+      <c r="H63" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69280,7 +69273,7 @@
       <c r="G64" s="23" t="n">
         <v>1.48462</v>
       </c>
-      <c r="H64" s="24" t="s">
+      <c r="H64" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69306,7 +69299,7 @@
       <c r="G65" s="23" t="n">
         <v>1.48</v>
       </c>
-      <c r="H65" s="24" t="s">
+      <c r="H65" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69332,7 +69325,7 @@
       <c r="G66" s="23" t="n">
         <v>1.47469</v>
       </c>
-      <c r="H66" s="24" t="s">
+      <c r="H66" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69358,7 +69351,7 @@
       <c r="G67" s="23" t="n">
         <v>1.46978</v>
       </c>
-      <c r="H67" s="24" t="s">
+      <c r="H67" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69384,7 +69377,7 @@
       <c r="G68" s="23" t="n">
         <v>1.46685</v>
       </c>
-      <c r="H68" s="24" t="s">
+      <c r="H68" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69410,7 +69403,7 @@
       <c r="G69" s="23" t="n">
         <v>1.46028</v>
       </c>
-      <c r="H69" s="24" t="s">
+      <c r="H69" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69436,7 +69429,7 @@
       <c r="G70" s="23" t="n">
         <v>1.45899</v>
       </c>
-      <c r="H70" s="24" t="s">
+      <c r="H70" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69462,7 +69455,7 @@
       <c r="G71" s="23" t="n">
         <v>1.45039</v>
       </c>
-      <c r="H71" s="24" t="s">
+      <c r="H71" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69488,7 +69481,7 @@
       <c r="G72" s="23" t="n">
         <v>1.44903</v>
       </c>
-      <c r="H72" s="24" t="s">
+      <c r="H72" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69514,7 +69507,7 @@
       <c r="G73" s="23" t="n">
         <v>1.44772</v>
       </c>
-      <c r="H73" s="24" t="s">
+      <c r="H73" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69540,7 +69533,7 @@
       <c r="G74" s="23" t="n">
         <v>1.44635</v>
       </c>
-      <c r="H74" s="24" t="s">
+      <c r="H74" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69566,7 +69559,7 @@
       <c r="G75" s="23" t="n">
         <v>1.44524</v>
       </c>
-      <c r="H75" s="24" t="s">
+      <c r="H75" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69592,7 +69585,7 @@
       <c r="G76" s="23" t="n">
         <v>1.44444</v>
       </c>
-      <c r="H76" s="24" t="s">
+      <c r="H76" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69618,7 +69611,7 @@
       <c r="G77" s="23" t="n">
         <v>1.44307</v>
       </c>
-      <c r="H77" s="24" t="s">
+      <c r="H77" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -69644,7 +69637,7 @@
       <c r="G78" s="23" t="n">
         <v>1.45607</v>
       </c>
-      <c r="H78" s="24" t="s">
+      <c r="H78" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69670,7 +69663,7 @@
       <c r="G79" s="23" t="n">
         <v>1.4567</v>
       </c>
-      <c r="H79" s="24" t="s">
+      <c r="H79" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69696,7 +69689,7 @@
       <c r="G80" s="23" t="n">
         <v>1.45846</v>
       </c>
-      <c r="H80" s="24" t="s">
+      <c r="H80" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69722,7 +69715,7 @@
       <c r="G81" s="23" t="n">
         <v>1.46186</v>
       </c>
-      <c r="H81" s="24" t="s">
+      <c r="H81" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69748,7 +69741,7 @@
       <c r="G82" s="23" t="n">
         <v>1.46224</v>
       </c>
-      <c r="H82" s="24" t="s">
+      <c r="H82" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69774,7 +69767,7 @@
       <c r="G83" s="23" t="n">
         <v>1.4635</v>
       </c>
-      <c r="H83" s="24" t="s">
+      <c r="H83" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69800,7 +69793,7 @@
       <c r="G84" s="23" t="n">
         <v>1.46406</v>
       </c>
-      <c r="H84" s="24" t="s">
+      <c r="H84" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69826,7 +69819,7 @@
       <c r="G85" s="23" t="n">
         <v>1.46429</v>
       </c>
-      <c r="H85" s="24" t="s">
+      <c r="H85" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69852,7 +69845,7 @@
       <c r="G86" s="23" t="n">
         <v>1.46669</v>
       </c>
-      <c r="H86" s="24" t="s">
+      <c r="H86" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -69878,7 +69871,7 @@
       <c r="G87" s="23" t="n">
         <v>1.46962</v>
       </c>
-      <c r="H87" s="24" t="s">
+      <c r="H87" s="12" t="s">
         <v>264</v>
       </c>
     </row>
@@ -72105,8 +72098,7 @@
       <c r="A173" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B173" s="14" t="n">
-        <f aca="false">100-C173-D173</f>
+      <c r="B173" s="5" t="n">
         <v>51.6663752450009</v>
       </c>
       <c r="C173" s="14" t="n">
@@ -72132,15 +72124,14 @@
       <c r="A174" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B174" s="14" t="n">
-        <f aca="false">100-C174-D174</f>
-        <v>5.72754916976213</v>
+      <c r="B174" s="5" t="n">
+        <v>52.7716789242694</v>
       </c>
       <c r="C174" s="14" t="n">
-        <v>3.37513100522291</v>
+        <v>4.30455048955563</v>
       </c>
       <c r="D174" s="14" t="n">
-        <v>90.897319825015</v>
+        <v>42.923770586175</v>
       </c>
       <c r="E174" s="14" t="n">
         <v>0</v>
@@ -72159,8 +72150,7 @@
       <c r="A175" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B175" s="14" t="n">
-        <f aca="false">100-C175-D175</f>
+      <c r="B175" s="5" t="n">
         <v>53.0084182186197</v>
       </c>
       <c r="C175" s="14" t="n">
@@ -72186,15 +72176,14 @@
       <c r="A176" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B176" s="14" t="n">
-        <f aca="false">100-C176-D176</f>
-        <v>51.5691526788673</v>
+      <c r="B176" s="5" t="n">
+        <v>53.6470788089306</v>
       </c>
       <c r="C176" s="14" t="n">
-        <v>6.21144054332535</v>
+        <v>5.94493860655915</v>
       </c>
       <c r="D176" s="14" t="n">
-        <v>42.2194067778073</v>
+        <v>40.4079825845103</v>
       </c>
       <c r="E176" s="14" t="n">
         <v>0</v>
@@ -72213,15 +72202,14 @@
       <c r="A177" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B177" s="14" t="n">
-        <f aca="false">100-C177-D177</f>
-        <v>0</v>
+      <c r="B177" s="5" t="n">
+        <v>52.7184664529172</v>
       </c>
       <c r="C177" s="14" t="n">
-        <v>6.29315830022271</v>
+        <v>2.97550175289083</v>
       </c>
       <c r="D177" s="14" t="n">
-        <v>93.7068416997773</v>
+        <v>44.306031794192</v>
       </c>
       <c r="E177" s="14" t="n">
         <v>0</v>
@@ -72240,9 +72228,8 @@
       <c r="A178" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B178" s="14" t="n">
-        <f aca="false">100-C178-D178</f>
-        <v>58.2221522713493</v>
+      <c r="B178" s="5" t="n">
+        <v>58.2221522713492</v>
       </c>
       <c r="C178" s="14" t="n">
         <v>6.10423577207711</v>
@@ -72267,8 +72254,7 @@
       <c r="A179" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B179" s="14" t="n">
-        <f aca="false">100-C179-D179</f>
+      <c r="B179" s="5" t="n">
         <v>57.8730320876436</v>
       </c>
       <c r="C179" s="14" t="n">
@@ -72294,8 +72280,7 @@
       <c r="A180" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B180" s="14" t="n">
-        <f aca="false">100-C180-D180</f>
+      <c r="B180" s="5" t="n">
         <v>58.6112473839572</v>
       </c>
       <c r="C180" s="14" t="n">
@@ -72321,8 +72306,7 @@
       <c r="A181" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B181" s="14" t="n">
-        <f aca="false">100-C181-D181</f>
+      <c r="B181" s="5" t="n">
         <v>57.1990820101673</v>
       </c>
       <c r="C181" s="14" t="n">
@@ -72348,8 +72332,7 @@
       <c r="A182" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B182" s="14" t="n">
-        <f aca="false">100-C182-D182</f>
+      <c r="B182" s="5" t="n">
         <v>57.7791097586646</v>
       </c>
       <c r="C182" s="14" t="n">
@@ -72375,8 +72358,7 @@
       <c r="A183" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B183" s="14" t="n">
-        <f aca="false">100-C183-D183</f>
+      <c r="B183" s="5" t="n">
         <v>63.5978989769</v>
       </c>
       <c r="C183" s="14" t="n">
@@ -72402,8 +72384,7 @@
       <c r="A184" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B184" s="14" t="n">
-        <f aca="false">100-C184-D184</f>
+      <c r="B184" s="5" t="n">
         <v>62.58864600015</v>
       </c>
       <c r="C184" s="14" t="n">
@@ -72429,8 +72410,7 @@
       <c r="A185" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B185" s="14" t="n">
-        <f aca="false">100-C185-D185</f>
+      <c r="B185" s="5" t="n">
         <v>62.1722776240317</v>
       </c>
       <c r="C185" s="14" t="n">
@@ -72456,8 +72436,7 @@
       <c r="A186" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B186" s="14" t="n">
-        <f aca="false">100-C186-D186</f>
+      <c r="B186" s="5" t="n">
         <v>61.7766318859742</v>
       </c>
       <c r="C186" s="14" t="n">
@@ -72483,8 +72462,7 @@
       <c r="A187" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B187" s="14" t="n">
-        <f aca="false">100-C187-D187</f>
+      <c r="B187" s="5" t="n">
         <v>63.9774744214685</v>
       </c>
       <c r="C187" s="14" t="n">
@@ -72510,8 +72488,7 @@
       <c r="A188" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B188" s="14" t="n">
-        <f aca="false">100-C188-D188</f>
+      <c r="B188" s="5" t="n">
         <v>63.3064519834963</v>
       </c>
       <c r="C188" s="14" t="n">
@@ -72537,8 +72514,7 @@
       <c r="A189" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B189" s="14" t="n">
-        <f aca="false">100-C189-D189</f>
+      <c r="B189" s="5" t="n">
         <v>65.7427340821742</v>
       </c>
       <c r="C189" s="14" t="n">
@@ -72564,8 +72540,7 @@
       <c r="A190" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B190" s="14" t="n">
-        <f aca="false">100-C190-D190</f>
+      <c r="B190" s="5" t="n">
         <v>68.4205607666823</v>
       </c>
       <c r="C190" s="14" t="n">
@@ -72591,8 +72566,7 @@
       <c r="A191" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B191" s="14" t="n">
-        <f aca="false">100-C191-D191</f>
+      <c r="B191" s="5" t="n">
         <v>67.6303285723881</v>
       </c>
       <c r="C191" s="14" t="n">
@@ -72618,8 +72592,7 @@
       <c r="A192" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B192" s="14" t="n">
-        <f aca="false">100-C192-D192</f>
+      <c r="B192" s="5" t="n">
         <v>69.0767608460237</v>
       </c>
       <c r="C192" s="14" t="n">
@@ -72645,8 +72618,7 @@
       <c r="A193" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B193" s="14" t="n">
-        <f aca="false">100-C193-D193</f>
+      <c r="B193" s="5" t="n">
         <v>67.3365841330101</v>
       </c>
       <c r="C193" s="14" t="n">
@@ -72672,8 +72644,7 @@
       <c r="A194" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B194" s="14" t="n">
-        <f aca="false">100-C194-D194</f>
+      <c r="B194" s="5" t="n">
         <v>67.236461025396</v>
       </c>
       <c r="C194" s="14" t="n">
@@ -72699,9 +72670,8 @@
       <c r="A195" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B195" s="14" t="n">
-        <f aca="false">100-C195-D195</f>
-        <v>67.5764087099867</v>
+      <c r="B195" s="5" t="n">
+        <v>67.5764087099868</v>
       </c>
       <c r="C195" s="14" t="n">
         <v>1.21816628877936</v>
@@ -72726,8 +72696,7 @@
       <c r="A196" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B196" s="14" t="n">
-        <f aca="false">100-C196-D196</f>
+      <c r="B196" s="5" t="n">
         <v>69.0707881494664</v>
       </c>
       <c r="C196" s="14" t="n">
@@ -72753,8 +72722,7 @@
       <c r="A197" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B197" s="14" t="n">
-        <f aca="false">100-C197-D197</f>
+      <c r="B197" s="5" t="n">
         <v>69.2084271715536</v>
       </c>
       <c r="C197" s="14" t="n">
@@ -72780,8 +72748,7 @@
       <c r="A198" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B198" s="14" t="n">
-        <f aca="false">100-C198-D198</f>
+      <c r="B198" s="5" t="n">
         <v>70.600069125291</v>
       </c>
       <c r="C198" s="14" t="n">
@@ -72807,8 +72774,7 @@
       <c r="A199" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B199" s="14" t="n">
-        <f aca="false">100-C199-D199</f>
+      <c r="B199" s="5" t="n">
         <v>71.0154500381631</v>
       </c>
       <c r="C199" s="14" t="n">
@@ -72834,8 +72800,7 @@
       <c r="A200" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B200" s="14" t="n">
-        <f aca="false">100-C200-D200</f>
+      <c r="B200" s="5" t="n">
         <v>70.9018860456718</v>
       </c>
       <c r="C200" s="14" t="n">
@@ -72861,8 +72826,7 @@
       <c r="A201" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B201" s="14" t="n">
-        <f aca="false">100-C201-D201</f>
+      <c r="B201" s="5" t="n">
         <v>71.3119017554588</v>
       </c>
       <c r="C201" s="14" t="n">
@@ -72888,8 +72852,7 @@
       <c r="A202" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B202" s="14" t="n">
-        <f aca="false">100-C202-D202</f>
+      <c r="B202" s="5" t="n">
         <v>72.291957164102</v>
       </c>
       <c r="C202" s="14" t="n">
@@ -72915,8 +72878,7 @@
       <c r="A203" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B203" s="14" t="n">
-        <f aca="false">100-C203-D203</f>
+      <c r="B203" s="5" t="n">
         <v>72.640810409275</v>
       </c>
       <c r="C203" s="14" t="n">
@@ -72942,8 +72904,7 @@
       <c r="A204" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B204" s="14" t="n">
-        <f aca="false">100-C204-D204</f>
+      <c r="B204" s="5" t="n">
         <v>72.2671487141094</v>
       </c>
       <c r="C204" s="14" t="n">
@@ -72969,8 +72930,7 @@
       <c r="A205" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B205" s="14" t="n">
-        <f aca="false">100-C205-D205</f>
+      <c r="B205" s="5" t="n">
         <v>73.3423595109387</v>
       </c>
       <c r="C205" s="14" t="n">
@@ -72996,8 +72956,7 @@
       <c r="A206" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B206" s="14" t="n">
-        <f aca="false">100-C206-D206</f>
+      <c r="B206" s="5" t="n">
         <v>74.3725179758444</v>
       </c>
       <c r="C206" s="14" t="n">
@@ -73023,15 +72982,14 @@
       <c r="A207" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B207" s="14" t="n">
-        <f aca="false">100-C207-D207</f>
+      <c r="B207" s="5" t="n">
         <v>74.0334613518314</v>
       </c>
       <c r="C207" s="14" t="n">
         <v>0.584469171060624</v>
       </c>
       <c r="D207" s="14" t="n">
-        <v>25.382069477108</v>
+        <v>25.3820694771079</v>
       </c>
       <c r="E207" s="14" t="n">
         <v>0</v>
@@ -73050,9 +73008,8 @@
       <c r="A208" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B208" s="14" t="n">
-        <f aca="false">100-C208-D208</f>
-        <v>75.7674606449692</v>
+      <c r="B208" s="5" t="n">
+        <v>75.7674606449693</v>
       </c>
       <c r="C208" s="14" t="n">
         <v>2.83701856541717</v>
@@ -73077,8 +73034,7 @@
       <c r="A209" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B209" s="14" t="n">
-        <f aca="false">100-C209-D209</f>
+      <c r="B209" s="5" t="n">
         <v>75.6153546658523</v>
       </c>
       <c r="C209" s="14" t="n">
@@ -73104,8 +73060,7 @@
       <c r="A210" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B210" s="14" t="n">
-        <f aca="false">100-C210-D210</f>
+      <c r="B210" s="5" t="n">
         <v>76.3367706380343</v>
       </c>
       <c r="C210" s="14" t="n">
@@ -73131,8 +73086,7 @@
       <c r="A211" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B211" s="14" t="n">
-        <f aca="false">100-C211-D211</f>
+      <c r="B211" s="5" t="n">
         <v>75.8392273419884</v>
       </c>
       <c r="C211" s="14" t="n">
@@ -73158,8 +73112,7 @@
       <c r="A212" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B212" s="14" t="n">
-        <f aca="false">100-C212-D212</f>
+      <c r="B212" s="5" t="n">
         <v>76.141260452542</v>
       </c>
       <c r="C212" s="14" t="n">
@@ -73185,8 +73138,7 @@
       <c r="A213" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B213" s="14" t="n">
-        <f aca="false">100-C213-D213</f>
+      <c r="B213" s="5" t="n">
         <v>77.3003396345546</v>
       </c>
       <c r="C213" s="14" t="n">
@@ -73212,8 +73164,7 @@
       <c r="A214" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B214" s="14" t="n">
-        <f aca="false">100-C214-D214</f>
+      <c r="B214" s="5" t="n">
         <v>77.480452479275</v>
       </c>
       <c r="C214" s="14" t="n">
@@ -73239,8 +73190,7 @@
       <c r="A215" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B215" s="14" t="n">
-        <f aca="false">100-C215-D215</f>
+      <c r="B215" s="5" t="n">
         <v>77.0186787060001</v>
       </c>
       <c r="C215" s="14" t="n">
@@ -73266,8 +73216,7 @@
       <c r="A216" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B216" s="14" t="n">
-        <f aca="false">100-C216-D216</f>
+      <c r="B216" s="5" t="n">
         <v>78.5226502475569</v>
       </c>
       <c r="C216" s="14" t="n">
@@ -73399,7 +73348,7 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="11" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="B221" s="14" t="n">
         <f aca="false">100-D221</f>
@@ -73826,7 +73775,7 @@
         <v>1.483</v>
       </c>
       <c r="H236" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73853,7 +73802,7 @@
         <v>1.486</v>
       </c>
       <c r="H237" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73880,7 +73829,7 @@
         <v>1.489</v>
       </c>
       <c r="H238" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73907,7 +73856,7 @@
         <v>1.494</v>
       </c>
       <c r="H239" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73934,7 +73883,7 @@
         <v>1.479</v>
       </c>
       <c r="H240" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73961,7 +73910,7 @@
         <v>1.4851</v>
       </c>
       <c r="H241" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -73988,7 +73937,7 @@
         <v>1.4898</v>
       </c>
       <c r="H242" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74015,7 +73964,7 @@
         <v>1.4912</v>
       </c>
       <c r="H243" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74042,7 +73991,7 @@
         <v>1.4925</v>
       </c>
       <c r="H244" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74069,7 +74018,7 @@
         <v>1.4965</v>
       </c>
       <c r="H245" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74096,7 +74045,7 @@
         <v>1.4993</v>
       </c>
       <c r="H246" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74123,7 +74072,7 @@
         <v>1.5015</v>
       </c>
       <c r="H247" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74150,7 +74099,7 @@
         <v>1.54014</v>
       </c>
       <c r="H248" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74177,7 +74126,7 @@
         <v>1.5021</v>
       </c>
       <c r="H249" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74204,7 +74153,7 @@
         <v>1.5042</v>
       </c>
       <c r="H250" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74231,7 +74180,7 @@
         <v>1.5055</v>
       </c>
       <c r="H251" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74258,7 +74207,7 @@
         <v>1.5055</v>
       </c>
       <c r="H252" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74285,7 +74234,7 @@
         <v>1.5075</v>
       </c>
       <c r="H253" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74312,7 +74261,7 @@
         <v>1.5076</v>
       </c>
       <c r="H254" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74339,7 +74288,7 @@
         <v>1.5099</v>
       </c>
       <c r="H255" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74366,7 +74315,7 @@
         <v>1.5112</v>
       </c>
       <c r="H256" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74393,7 +74342,7 @@
         <v>1.5137</v>
       </c>
       <c r="H257" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74420,7 +74369,7 @@
         <v>1.515</v>
       </c>
       <c r="H258" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74447,7 +74396,7 @@
         <v>1.5146</v>
       </c>
       <c r="H259" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74474,7 +74423,7 @@
         <v>1.5163</v>
       </c>
       <c r="H260" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74501,7 +74450,7 @@
         <v>1.4822</v>
       </c>
       <c r="H261" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74528,7 +74477,7 @@
         <v>1.4906</v>
       </c>
       <c r="H262" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74555,7 +74504,7 @@
         <v>1.4983</v>
       </c>
       <c r="H263" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74581,7 +74530,7 @@
         <v>1.5041</v>
       </c>
       <c r="H264" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74607,7 +74556,7 @@
         <v>1.5061</v>
       </c>
       <c r="H265" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74634,7 +74583,7 @@
         <v>1.482</v>
       </c>
       <c r="H266" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74661,7 +74610,7 @@
         <v>1.486</v>
       </c>
       <c r="H267" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74688,7 +74637,7 @@
         <v>1.49</v>
       </c>
       <c r="H268" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74715,7 +74664,7 @@
         <v>1.496</v>
       </c>
       <c r="H269" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74742,7 +74691,7 @@
         <v>1.5</v>
       </c>
       <c r="H270" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74769,7 +74718,7 @@
         <v>1.504</v>
       </c>
       <c r="H271" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74796,7 +74745,7 @@
         <v>1.508</v>
       </c>
       <c r="H272" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74823,7 +74772,7 @@
         <v>1.52</v>
       </c>
       <c r="H273" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74850,7 +74799,7 @@
         <v>1.469</v>
       </c>
       <c r="H274" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74877,7 +74826,7 @@
         <v>1.477</v>
       </c>
       <c r="H275" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74904,7 +74853,7 @@
         <v>1.481</v>
       </c>
       <c r="H276" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74931,7 +74880,7 @@
         <v>1.486</v>
       </c>
       <c r="H277" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74958,7 +74907,7 @@
         <v>1.495</v>
       </c>
       <c r="H278" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -74985,7 +74934,7 @@
         <v>1.502</v>
       </c>
       <c r="H279" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75012,12 +74961,12 @@
         <v>1.51</v>
       </c>
       <c r="H280" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B281" s="14" t="n">
         <f aca="false">100-C281</f>
@@ -75039,18 +74988,18 @@
         <v>1.478</v>
       </c>
       <c r="H281" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B282" s="14" t="n">
         <f aca="false">100-C282</f>
         <v>80</v>
       </c>
-      <c r="C282" s="22" t="n">
+      <c r="C282" s="14" t="n">
         <v>20</v>
       </c>
       <c r="D282" s="14" t="n">
@@ -75066,18 +75015,18 @@
         <v>1.504</v>
       </c>
       <c r="H282" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B283" s="14" t="n">
         <f aca="false">100-C283</f>
         <v>67</v>
       </c>
-      <c r="C283" s="22" t="n">
+      <c r="C283" s="14" t="n">
         <v>33</v>
       </c>
       <c r="D283" s="14" t="n">
@@ -75093,12 +75042,12 @@
         <v>1.535</v>
       </c>
       <c r="H283" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B284" s="14" t="n">
         <f aca="false">100-C284</f>
@@ -75120,12 +75069,12 @@
         <v>1.574</v>
       </c>
       <c r="H284" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B285" s="14" t="n">
         <f aca="false">100-C285</f>
@@ -75147,12 +75096,12 @@
         <v>1.597</v>
       </c>
       <c r="H285" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B286" s="14" t="n">
         <f aca="false">100-C286</f>
@@ -75174,12 +75123,12 @@
         <v>1.629</v>
       </c>
       <c r="H286" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B287" s="14" t="n">
         <f aca="false">100-C287</f>
@@ -75201,12 +75150,12 @@
         <v>1.634</v>
       </c>
       <c r="H287" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B288" s="14" t="n">
         <f aca="false">100-C288</f>
@@ -75228,12 +75177,12 @@
         <v>1.72</v>
       </c>
       <c r="H288" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B289" s="14" t="n">
         <f aca="false">100-C289</f>
@@ -75255,7 +75204,7 @@
         <v>1.728</v>
       </c>
       <c r="H289" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75282,7 +75231,7 @@
         <v>1.499</v>
       </c>
       <c r="H290" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75309,7 +75258,7 @@
         <v>1.499</v>
       </c>
       <c r="H291" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75336,7 +75285,7 @@
         <v>1.5</v>
       </c>
       <c r="H292" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75363,7 +75312,7 @@
         <v>1.5</v>
       </c>
       <c r="H293" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75390,7 +75339,7 @@
         <v>1.5</v>
       </c>
       <c r="H294" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75417,7 +75366,7 @@
         <v>1.501</v>
       </c>
       <c r="H295" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75444,7 +75393,7 @@
         <v>1.501</v>
       </c>
       <c r="H296" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75471,7 +75420,7 @@
         <v>1.499</v>
       </c>
       <c r="H297" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75498,7 +75447,7 @@
         <v>1.499</v>
       </c>
       <c r="H298" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75525,7 +75474,7 @@
         <v>1.498</v>
       </c>
       <c r="H299" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75552,7 +75501,7 @@
         <v>1.498</v>
       </c>
       <c r="H300" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75579,7 +75528,7 @@
         <v>1.498</v>
       </c>
       <c r="H301" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75606,7 +75555,7 @@
         <v>1.4989</v>
       </c>
       <c r="H302" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75633,7 +75582,7 @@
         <v>1.499</v>
       </c>
       <c r="H303" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75660,7 +75609,7 @@
         <v>1.499</v>
       </c>
       <c r="H304" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75687,7 +75636,7 @@
         <v>1.498</v>
       </c>
       <c r="H305" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75714,7 +75663,7 @@
         <v>1.4985</v>
       </c>
       <c r="H306" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75741,7 +75690,7 @@
         <v>1.498</v>
       </c>
       <c r="H307" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75768,7 +75717,7 @@
         <v>1.4965</v>
       </c>
       <c r="H308" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75795,7 +75744,7 @@
         <v>1.4962</v>
       </c>
       <c r="H309" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75822,7 +75771,7 @@
         <v>1.497</v>
       </c>
       <c r="H310" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75849,7 +75798,7 @@
         <v>1.4959</v>
       </c>
       <c r="H311" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75876,7 +75825,7 @@
         <v>1.4944</v>
       </c>
       <c r="H312" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75903,7 +75852,7 @@
         <v>1.4958</v>
       </c>
       <c r="H313" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75930,7 +75879,7 @@
         <v>1.4964</v>
       </c>
       <c r="H314" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75957,7 +75906,7 @@
         <v>1.4961</v>
       </c>
       <c r="H315" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -75984,7 +75933,7 @@
         <v>1.4946</v>
       </c>
       <c r="H316" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76011,7 +75960,7 @@
         <v>1.4937</v>
       </c>
       <c r="H317" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76038,7 +75987,7 @@
         <v>1.4929</v>
       </c>
       <c r="H318" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76065,7 +76014,7 @@
         <v>1.4946</v>
       </c>
       <c r="H319" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76092,7 +76041,7 @@
         <v>1.4938</v>
       </c>
       <c r="H320" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76119,7 +76068,7 @@
         <v>1.4936</v>
       </c>
       <c r="H321" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76146,7 +76095,7 @@
         <v>1.4922</v>
       </c>
       <c r="H322" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76173,7 +76122,7 @@
         <v>1.4927</v>
       </c>
       <c r="H323" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76200,7 +76149,7 @@
         <v>1.4923</v>
       </c>
       <c r="H324" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76227,7 +76176,7 @@
         <v>1.4912</v>
       </c>
       <c r="H325" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76254,7 +76203,7 @@
         <v>1.4902</v>
       </c>
       <c r="H326" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76281,7 +76230,7 @@
         <v>1.4911</v>
       </c>
       <c r="H327" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76308,7 +76257,7 @@
         <v>1.491</v>
       </c>
       <c r="H328" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76335,7 +76284,7 @@
         <v>1.4895</v>
       </c>
       <c r="H329" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76362,7 +76311,7 @@
         <v>1.4883</v>
       </c>
       <c r="H330" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76389,7 +76338,7 @@
         <v>1.4902</v>
       </c>
       <c r="H331" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76416,7 +76365,7 @@
         <v>1.4891</v>
       </c>
       <c r="H332" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76443,7 +76392,7 @@
         <v>1.4878</v>
       </c>
       <c r="H333" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76470,7 +76419,7 @@
         <v>1.4864</v>
       </c>
       <c r="H334" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76497,7 +76446,7 @@
         <v>1.4881</v>
       </c>
       <c r="H335" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76524,7 +76473,7 @@
         <v>1.4875</v>
       </c>
       <c r="H336" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76551,7 +76500,7 @@
         <v>1.486</v>
       </c>
       <c r="H337" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76578,7 +76527,7 @@
         <v>1.487</v>
       </c>
       <c r="H338" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76605,7 +76554,7 @@
         <v>1.4841</v>
       </c>
       <c r="H339" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76632,7 +76581,7 @@
         <v>1.4848</v>
       </c>
       <c r="H340" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -76659,7 +76608,7 @@
         <v>1.4813</v>
       </c>
       <c r="H341" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -76688,57 +76637,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="26.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="12.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="10.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="25" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="26.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="10.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="24" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.33"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+    <row r="1" s="26" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="L1" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>288</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>289</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>514.532</v>
@@ -76767,16 +76716,16 @@
       <c r="K2" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>290</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>291</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>514.532</v>
@@ -76805,16 +76754,16 @@
       <c r="K3" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>292</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>293</v>
       </c>
       <c r="C4" s="12" t="n">
         <v>514.532</v>
@@ -76843,16 +76792,16 @@
       <c r="K4" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>294</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>295</v>
       </c>
       <c r="C5" s="12" t="n">
         <v>514.532</v>
@@ -76881,15 +76830,15 @@
       <c r="K5" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
-        <v>296</v>
-      </c>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="12" t="n">
@@ -76919,15 +76868,15 @@
       <c r="K6" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="s">
-        <v>297</v>
-      </c>
-      <c r="B7" s="28" t="s">
+      <c r="A7" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>234</v>
       </c>
       <c r="C7" s="12" t="n">
@@ -76957,16 +76906,16 @@
       <c r="K7" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>298</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>299</v>
       </c>
       <c r="C8" s="12" t="n">
         <v>514.532</v>
@@ -76995,16 +76944,16 @@
       <c r="K8" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="L8" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>300</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>301</v>
       </c>
       <c r="C9" s="12" t="n">
         <v>514.532</v>
@@ -77033,16 +76982,16 @@
       <c r="K9" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="L9" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>302</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>303</v>
       </c>
       <c r="C10" s="12" t="n">
         <v>514.532</v>
@@ -77071,16 +77020,16 @@
       <c r="K10" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>304</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>305</v>
       </c>
       <c r="C11" s="12" t="n">
         <v>514.532</v>
@@ -77109,30 +77058,30 @@
       <c r="K11" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="L11" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
-        <v>302</v>
-      </c>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>216</v>
       </c>
       <c r="C12" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D12" s="29" t="n">
+      <c r="D12" s="28" t="n">
         <v>74.9745426640969</v>
       </c>
-      <c r="E12" s="30" t="n">
+      <c r="E12" s="29" t="n">
         <v>12.5324994764899</v>
       </c>
-      <c r="F12" s="30" t="n">
+      <c r="F12" s="29" t="n">
         <v>12.4929578594132</v>
       </c>
-      <c r="G12" s="30" t="n">
+      <c r="G12" s="29" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="12" t="n">
@@ -77147,16 +77096,16 @@
       <c r="K12" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="L12" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>306</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>307</v>
       </c>
       <c r="C13" s="12" t="n">
         <v>514.532</v>
@@ -77185,16 +77134,16 @@
       <c r="K13" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>308</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>309</v>
       </c>
       <c r="C14" s="12" t="n">
         <v>514.532</v>
@@ -77223,16 +77172,16 @@
       <c r="K14" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L14" s="25" t="s">
+      <c r="L14" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>310</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>311</v>
       </c>
       <c r="C15" s="12" t="n">
         <v>514.532</v>
@@ -77261,15 +77210,15 @@
       <c r="K15" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="L15" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="B16" s="28" t="s">
+      <c r="A16" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>235</v>
       </c>
       <c r="C16" s="12" t="n">
@@ -77299,15 +77248,15 @@
       <c r="K16" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="L16" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="B17" s="28" t="s">
+      <c r="A17" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>236</v>
       </c>
       <c r="C17" s="12" t="n">
@@ -77337,15 +77286,15 @@
       <c r="K17" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="L17" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25" t="s">
-        <v>314</v>
-      </c>
-      <c r="B18" s="28" t="s">
+      <c r="A18" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>237</v>
       </c>
       <c r="C18" s="12" t="n">
@@ -77375,15 +77324,15 @@
       <c r="K18" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L18" s="25" t="s">
+      <c r="L18" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="B19" s="28" t="s">
+      <c r="A19" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>238</v>
       </c>
       <c r="C19" s="12" t="n">
@@ -77413,15 +77362,15 @@
       <c r="K19" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="L19" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25" t="s">
-        <v>316</v>
-      </c>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>239</v>
       </c>
       <c r="C20" s="12" t="n">
@@ -77451,15 +77400,15 @@
       <c r="K20" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L20" s="25" t="s">
+      <c r="L20" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="B21" s="28" t="s">
+      <c r="A21" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>229</v>
       </c>
       <c r="C21" s="12" t="n">
@@ -77489,15 +77438,15 @@
       <c r="K21" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L21" s="25" t="s">
+      <c r="L21" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="s">
-        <v>318</v>
-      </c>
-      <c r="B22" s="28" t="s">
+      <c r="A22" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>231</v>
       </c>
       <c r="C22" s="12" t="n">
@@ -77527,15 +77476,15 @@
       <c r="K22" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L22" s="25" t="s">
+      <c r="L22" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="s">
-        <v>319</v>
-      </c>
-      <c r="B23" s="28" t="s">
+      <c r="A23" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>232</v>
       </c>
       <c r="C23" s="12" t="n">
@@ -77565,15 +77514,15 @@
       <c r="K23" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L23" s="25" t="s">
+      <c r="L23" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="B24" s="28" t="s">
+      <c r="A24" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>233</v>
       </c>
       <c r="C24" s="12" t="n">
@@ -77603,15 +77552,15 @@
       <c r="K24" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L24" s="25" t="s">
+      <c r="L24" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="25" t="s">
-        <v>321</v>
-      </c>
-      <c r="B25" s="28" t="s">
+      <c r="A25" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>230</v>
       </c>
       <c r="C25" s="12" t="n">
@@ -77641,30 +77590,30 @@
       <c r="K25" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L25" s="25" t="s">
+      <c r="L25" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25" t="s">
-        <v>322</v>
-      </c>
-      <c r="B26" s="28" t="s">
+      <c r="A26" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>217</v>
       </c>
       <c r="C26" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D26" s="29" t="n">
+      <c r="D26" s="28" t="n">
         <v>75.3671748325506</v>
       </c>
-      <c r="E26" s="30" t="n">
+      <c r="E26" s="29" t="n">
         <v>12.5101810960938</v>
       </c>
-      <c r="F26" s="30" t="n">
+      <c r="F26" s="29" t="n">
         <v>9.74972150865375</v>
       </c>
-      <c r="G26" s="30" t="n">
+      <c r="G26" s="29" t="n">
         <v>2.37292256270181</v>
       </c>
       <c r="H26" s="12" t="n">
@@ -77679,30 +77628,30 @@
       <c r="K26" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L26" s="25" t="s">
+      <c r="L26" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="B27" s="28" t="s">
+      <c r="A27" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>218</v>
       </c>
       <c r="C27" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D27" s="29" t="n">
+      <c r="D27" s="28" t="n">
         <v>75.3325352579704</v>
       </c>
-      <c r="E27" s="30" t="n">
+      <c r="E27" s="29" t="n">
         <v>12.440304702182</v>
       </c>
-      <c r="F27" s="30" t="n">
+      <c r="F27" s="29" t="n">
         <v>7.43508173818021</v>
       </c>
-      <c r="G27" s="30" t="n">
+      <c r="G27" s="29" t="n">
         <v>4.79207830166733</v>
       </c>
       <c r="H27" s="12" t="n">
@@ -77717,30 +77666,30 @@
       <c r="K27" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L27" s="25" t="s">
+      <c r="L27" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="25" t="s">
-        <v>324</v>
-      </c>
-      <c r="B28" s="28" t="s">
+      <c r="A28" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>219</v>
       </c>
       <c r="C28" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D28" s="29" t="n">
+      <c r="D28" s="28" t="n">
         <v>75.1585036363751</v>
       </c>
-      <c r="E28" s="30" t="n">
+      <c r="E28" s="29" t="n">
         <v>12.5039020562326</v>
       </c>
-      <c r="F28" s="30" t="n">
+      <c r="F28" s="29" t="n">
         <v>6.14811933249659</v>
       </c>
-      <c r="G28" s="30" t="n">
+      <c r="G28" s="29" t="n">
         <v>6.18947497489577</v>
       </c>
       <c r="H28" s="12" t="n">
@@ -77755,30 +77704,30 @@
       <c r="K28" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L28" s="25" t="s">
+      <c r="L28" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25" t="s">
-        <v>325</v>
-      </c>
-      <c r="B29" s="28" t="s">
+      <c r="A29" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>220</v>
       </c>
       <c r="C29" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D29" s="29" t="n">
+      <c r="D29" s="28" t="n">
         <v>75.5348273464621</v>
       </c>
-      <c r="E29" s="30" t="n">
+      <c r="E29" s="29" t="n">
         <v>12.304676320589</v>
       </c>
-      <c r="F29" s="30" t="n">
+      <c r="F29" s="29" t="n">
         <v>5.00862797129772</v>
       </c>
-      <c r="G29" s="30" t="n">
+      <c r="G29" s="29" t="n">
         <v>7.15186836165118</v>
       </c>
       <c r="H29" s="12" t="n">
@@ -77793,30 +77742,30 @@
       <c r="K29" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L29" s="25" t="s">
+      <c r="L29" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="25" t="s">
-        <v>326</v>
-      </c>
-      <c r="B30" s="28" t="s">
+      <c r="A30" s="24" t="s">
+        <v>325</v>
+      </c>
+      <c r="B30" s="27" t="s">
         <v>221</v>
       </c>
       <c r="C30" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D30" s="29" t="n">
+      <c r="D30" s="28" t="n">
         <v>75.1517851484335</v>
       </c>
-      <c r="E30" s="30" t="n">
+      <c r="E30" s="29" t="n">
         <v>12.4271601120841</v>
       </c>
-      <c r="F30" s="30" t="n">
+      <c r="F30" s="29" t="n">
         <v>2.65935482146804</v>
       </c>
-      <c r="G30" s="30" t="n">
+      <c r="G30" s="29" t="n">
         <v>9.76169991801431</v>
       </c>
       <c r="H30" s="12" t="n">
@@ -77831,30 +77780,30 @@
       <c r="K30" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L30" s="25" t="s">
+      <c r="L30" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25" t="s">
-        <v>327</v>
-      </c>
-      <c r="B31" s="28" t="s">
+      <c r="A31" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>222</v>
       </c>
       <c r="C31" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D31" s="29" t="n">
+      <c r="D31" s="28" t="n">
         <v>75.0616299962015</v>
       </c>
-      <c r="E31" s="30" t="n">
+      <c r="E31" s="29" t="n">
         <v>12.7521452301599</v>
       </c>
-      <c r="F31" s="30" t="n">
+      <c r="F31" s="29" t="n">
         <v>0.0897952692747758</v>
       </c>
-      <c r="G31" s="30" t="n">
+      <c r="G31" s="29" t="n">
         <v>12.0964295043637</v>
       </c>
       <c r="H31" s="12" t="n">
@@ -77869,30 +77818,30 @@
       <c r="K31" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L31" s="25" t="s">
+      <c r="L31" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="25" t="s">
-        <v>328</v>
-      </c>
-      <c r="B32" s="28" t="s">
+      <c r="A32" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>204</v>
       </c>
       <c r="C32" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D32" s="29" t="n">
+      <c r="D32" s="28" t="n">
         <v>83.9026344786137</v>
       </c>
-      <c r="E32" s="30" t="n">
+      <c r="E32" s="29" t="n">
         <v>8.74486627266353</v>
       </c>
-      <c r="F32" s="30" t="n">
+      <c r="F32" s="29" t="n">
         <v>7.35249924872283</v>
       </c>
-      <c r="G32" s="30" t="n">
+      <c r="G32" s="29" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="12" t="n">
@@ -77907,30 +77856,30 @@
       <c r="K32" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L32" s="25" t="s">
+      <c r="L32" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="B33" s="28" t="s">
+      <c r="A33" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="B33" s="27" t="s">
         <v>205</v>
       </c>
       <c r="C33" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D33" s="29" t="n">
+      <c r="D33" s="28" t="n">
         <v>83.4</v>
       </c>
-      <c r="E33" s="30" t="n">
+      <c r="E33" s="29" t="n">
         <v>8.33</v>
       </c>
-      <c r="F33" s="30" t="n">
+      <c r="F33" s="29" t="n">
         <v>6.21</v>
       </c>
-      <c r="G33" s="30" t="n">
+      <c r="G33" s="29" t="n">
         <v>2.06</v>
       </c>
       <c r="H33" s="12" t="n">
@@ -77945,30 +77894,30 @@
       <c r="K33" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L33" s="25" t="s">
+      <c r="L33" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="25" t="s">
-        <v>330</v>
-      </c>
-      <c r="B34" s="28" t="s">
+      <c r="A34" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>206</v>
       </c>
       <c r="C34" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D34" s="29" t="n">
+      <c r="D34" s="28" t="n">
         <v>83.23</v>
       </c>
-      <c r="E34" s="30" t="n">
+      <c r="E34" s="29" t="n">
         <v>8.42</v>
       </c>
-      <c r="F34" s="30" t="n">
+      <c r="F34" s="29" t="n">
         <v>4.21</v>
       </c>
-      <c r="G34" s="30" t="n">
+      <c r="G34" s="29" t="n">
         <v>4.14</v>
       </c>
       <c r="H34" s="12" t="n">
@@ -77983,30 +77932,30 @@
       <c r="K34" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L34" s="25" t="s">
+      <c r="L34" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="s">
-        <v>331</v>
-      </c>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="B35" s="27" t="s">
         <v>207</v>
       </c>
       <c r="C35" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D35" s="29" t="n">
+      <c r="D35" s="28" t="n">
         <v>83.27</v>
       </c>
-      <c r="E35" s="30" t="n">
+      <c r="E35" s="29" t="n">
         <v>8.48</v>
       </c>
-      <c r="F35" s="30" t="n">
+      <c r="F35" s="29" t="n">
         <v>2.19</v>
       </c>
-      <c r="G35" s="30" t="n">
+      <c r="G35" s="29" t="n">
         <v>6.06</v>
       </c>
       <c r="H35" s="12" t="n">
@@ -78021,30 +77970,30 @@
       <c r="K35" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L35" s="25" t="s">
+      <c r="L35" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="25" t="s">
-        <v>332</v>
-      </c>
-      <c r="B36" s="28" t="s">
+      <c r="A36" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="B36" s="27" t="s">
         <v>208</v>
       </c>
       <c r="C36" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D36" s="29" t="n">
+      <c r="D36" s="28" t="n">
         <v>83.1031031031031</v>
       </c>
-      <c r="E36" s="30" t="n">
+      <c r="E36" s="29" t="n">
         <v>8.5985985985986</v>
       </c>
-      <c r="F36" s="30" t="n">
+      <c r="F36" s="29" t="n">
         <v>0.12012012012012</v>
       </c>
-      <c r="G36" s="30" t="n">
+      <c r="G36" s="29" t="n">
         <v>8.17817817817818</v>
       </c>
       <c r="H36" s="12" t="n">
@@ -78059,30 +78008,30 @@
       <c r="K36" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L36" s="25" t="s">
+      <c r="L36" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="B37" s="27" t="s">
         <v>333</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>334</v>
       </c>
       <c r="C37" s="12" t="n">
         <v>514.532</v>
       </c>
-      <c r="D37" s="29" t="n">
+      <c r="D37" s="28" t="n">
         <v>90.0178159500554</v>
       </c>
-      <c r="E37" s="30" t="n">
+      <c r="E37" s="29" t="n">
         <v>5.00442961761284</v>
       </c>
-      <c r="F37" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" s="30" t="n">
+      <c r="F37" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="29" t="n">
         <v>4.9777544323318</v>
       </c>
       <c r="H37" s="12" t="n">
@@ -78097,15 +78046,15 @@
       <c r="K37" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L37" s="25" t="s">
+      <c r="L37" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="25" t="s">
-        <v>335</v>
-      </c>
-      <c r="B38" s="28" t="s">
+      <c r="A38" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="B38" s="27" t="s">
         <v>209</v>
       </c>
       <c r="C38" s="12" t="n">
@@ -78135,15 +78084,15 @@
       <c r="K38" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L38" s="25" t="s">
+      <c r="L38" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="25" t="s">
-        <v>336</v>
-      </c>
-      <c r="B39" s="28" t="s">
+      <c r="A39" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="B39" s="27" t="s">
         <v>224</v>
       </c>
       <c r="C39" s="12" t="n">
@@ -78173,16 +78122,16 @@
       <c r="K39" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L39" s="25" t="s">
+      <c r="L39" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="B40" s="27" t="s">
         <v>337</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>338</v>
       </c>
       <c r="C40" s="12" t="n">
         <v>514.532</v>
@@ -78211,16 +78160,16 @@
       <c r="K40" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L40" s="25" t="s">
+      <c r="L40" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="B41" s="27" t="s">
         <v>339</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>340</v>
       </c>
       <c r="C41" s="12" t="n">
         <v>514.532</v>
@@ -78249,16 +78198,16 @@
       <c r="K41" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L41" s="25" t="s">
+      <c r="L41" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="B42" s="27" t="s">
         <v>341</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>342</v>
       </c>
       <c r="C42" s="12" t="n">
         <v>488</v>
@@ -78287,16 +78236,16 @@
       <c r="K42" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L42" s="25" t="s">
+      <c r="L42" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="B43" s="27" t="s">
         <v>343</v>
-      </c>
-      <c r="B43" s="28" t="s">
-        <v>344</v>
       </c>
       <c r="C43" s="12" t="n">
         <v>488</v>
@@ -78325,16 +78274,16 @@
       <c r="K43" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L43" s="25" t="s">
+      <c r="L43" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="B44" s="27" t="s">
         <v>345</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>346</v>
       </c>
       <c r="C44" s="12" t="n">
         <v>488</v>
@@ -78363,16 +78312,16 @@
       <c r="K44" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L44" s="25" t="s">
+      <c r="L44" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="B45" s="27" t="s">
         <v>347</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>348</v>
       </c>
       <c r="C45" s="12" t="n">
         <v>488</v>
@@ -78401,16 +78350,16 @@
       <c r="K45" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L45" s="25" t="s">
+      <c r="L45" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="B46" s="27" t="s">
         <v>349</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>350</v>
       </c>
       <c r="C46" s="12" t="n">
         <v>488</v>
@@ -78439,16 +78388,16 @@
       <c r="K46" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L46" s="25" t="s">
+      <c r="L46" s="24" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="B47" s="24" t="s">
         <v>351</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>352</v>
       </c>
       <c r="C47" s="12" t="n">
         <v>488</v>
@@ -78477,16 +78426,16 @@
       <c r="K47" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L47" s="25" t="s">
+      <c r="L47" s="24" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="24" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="25" t="s">
-        <v>354</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>352</v>
+      <c r="B48" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C48" s="12" t="n">
         <v>488</v>
@@ -78515,16 +78464,16 @@
       <c r="K48" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L48" s="25" t="s">
-        <v>353</v>
+      <c r="L48" s="24" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="B49" s="25" t="s">
-        <v>352</v>
+      <c r="A49" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C49" s="12" t="n">
         <v>488</v>
@@ -78553,16 +78502,16 @@
       <c r="K49" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L49" s="25" t="s">
-        <v>353</v>
+      <c r="L49" s="24" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="25" t="s">
-        <v>356</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>352</v>
+      <c r="A50" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C50" s="12" t="n">
         <v>488</v>
@@ -78591,16 +78540,16 @@
       <c r="K50" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L50" s="25" t="s">
-        <v>353</v>
+      <c r="L50" s="24" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="25" t="s">
-        <v>357</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>352</v>
+      <c r="A51" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C51" s="12" t="n">
         <v>488</v>
@@ -78629,16 +78578,16 @@
       <c r="K51" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L51" s="25" t="s">
-        <v>353</v>
+      <c r="L51" s="24" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="25" t="s">
-        <v>358</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>352</v>
+      <c r="A52" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C52" s="12" t="n">
         <v>488</v>
@@ -78667,16 +78616,16 @@
       <c r="K52" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L52" s="25" t="s">
-        <v>353</v>
+      <c r="L52" s="24" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="25" t="s">
-        <v>359</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>352</v>
+      <c r="A53" s="24" t="s">
+        <v>358</v>
+      </c>
+      <c r="B53" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C53" s="12" t="n">
         <v>488</v>
@@ -78705,16 +78654,16 @@
       <c r="K53" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L53" s="25" t="s">
+      <c r="L53" s="24" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="24" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="25" t="s">
-        <v>361</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>352</v>
+      <c r="B54" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C54" s="12" t="n">
         <v>488</v>
@@ -78743,16 +78692,16 @@
       <c r="K54" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L54" s="25" t="s">
-        <v>360</v>
+      <c r="L54" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="25" t="s">
-        <v>362</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>352</v>
+      <c r="A55" s="24" t="s">
+        <v>361</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C55" s="12" t="n">
         <v>488</v>
@@ -78781,16 +78730,16 @@
       <c r="K55" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L55" s="25" t="s">
-        <v>360</v>
+      <c r="L55" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="25" t="s">
-        <v>363</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>352</v>
+      <c r="A56" s="24" t="s">
+        <v>362</v>
+      </c>
+      <c r="B56" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C56" s="12" t="n">
         <v>488</v>
@@ -78819,16 +78768,16 @@
       <c r="K56" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L56" s="25" t="s">
-        <v>360</v>
+      <c r="L56" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="25" t="s">
-        <v>364</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>352</v>
+      <c r="A57" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C57" s="12" t="n">
         <v>488</v>
@@ -78857,16 +78806,16 @@
       <c r="K57" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L57" s="25" t="s">
-        <v>360</v>
+      <c r="L57" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25" t="s">
-        <v>365</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>352</v>
+      <c r="A58" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="B58" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C58" s="12" t="n">
         <v>488</v>
@@ -78895,16 +78844,16 @@
       <c r="K58" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L58" s="25" t="s">
-        <v>360</v>
+      <c r="L58" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25" t="s">
-        <v>366</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>352</v>
+      <c r="A59" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C59" s="12" t="n">
         <v>488</v>
@@ -78933,16 +78882,16 @@
       <c r="K59" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L59" s="25" t="s">
-        <v>360</v>
+      <c r="L59" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>352</v>
+      <c r="A60" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C60" s="12" t="n">
         <v>488</v>
@@ -78971,16 +78920,16 @@
       <c r="K60" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L60" s="25" t="s">
-        <v>360</v>
+      <c r="L60" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="25" t="s">
-        <v>368</v>
-      </c>
-      <c r="B61" s="25" t="s">
-        <v>352</v>
+      <c r="A61" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C61" s="12" t="n">
         <v>488</v>
@@ -79009,16 +78958,16 @@
       <c r="K61" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L61" s="25" t="s">
-        <v>360</v>
+      <c r="L61" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>352</v>
+      <c r="A62" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="C62" s="12" t="n">
         <v>488</v>
@@ -79047,15 +78996,15 @@
       <c r="K62" s="12" t="n">
         <v>1500</v>
       </c>
-      <c r="L62" s="25" t="s">
-        <v>360</v>
+      <c r="L62" s="24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="25" t="s">
-        <v>370</v>
-      </c>
-      <c r="B63" s="25" t="s">
+      <c r="A63" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="B63" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C63" s="12" t="n">
@@ -79085,8 +79034,8 @@
       <c r="K63" s="12" t="n">
         <v>1400</v>
       </c>
-      <c r="L63" s="25" t="s">
-        <v>371</v>
+      <c r="L63" s="24" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -79108,53 +79057,54 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="2" style="0" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="B4" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
-        <v>261</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79162,55 +79112,55 @@
         <v>169</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>380</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>382</v>
+      <c r="B9" s="31" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>383</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>385</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79218,15 +79168,15 @@
         <v>268</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>389</v>
+      <c r="B15" s="31" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79234,7 +79184,7 @@
         <v>161</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79242,7 +79192,7 @@
         <v>171</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79250,7 +79200,7 @@
         <v>266</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79258,79 +79208,79 @@
         <v>103</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="30" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="32" t="s">
-        <v>395</v>
+      <c r="B21" s="31" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>396</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="32" t="s">
-        <v>398</v>
+      <c r="B23" s="31" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="32" t="s">
-        <v>399</v>
+      <c r="B24" s="31" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="32" t="s">
-        <v>400</v>
+      <c r="B25" s="31" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="B26" s="32" t="s">
-        <v>401</v>
+      <c r="B26" s="31" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79338,7 +79288,7 @@
         <v>269</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79346,23 +79296,23 @@
         <v>23</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>406</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>408</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79370,31 +79320,31 @@
         <v>265</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>411</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>413</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="32" t="s">
-        <v>415</v>
+      <c r="B36" s="31" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79402,7 +79352,7 @@
         <v>187</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79410,31 +79360,31 @@
         <v>267</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="B39" s="32" t="s">
-        <v>418</v>
+      <c r="B39" s="31" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79442,31 +79392,31 @@
         <v>124</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="33" t="s">
-        <v>424</v>
+      <c r="B46" s="32" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79474,7 +79424,7 @@
         <v>263</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79482,17 +79432,17 @@
         <v>264</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -79529,13 +79479,13 @@
         <v>6</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AA34" s="0" t="s">
         <v>6</v>
       </c>
       <c r="AB34" s="0" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79572,7 +79522,7 @@
       <c r="K35" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="34" t="n">
+      <c r="L35" s="33" t="n">
         <v>1671.43529428606</v>
       </c>
       <c r="M35" s="9" t="n">
@@ -79582,7 +79532,7 @@
         <v>103</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q35" s="6" t="n">
         <v>75</v>
@@ -79655,7 +79605,7 @@
       <c r="K36" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="34" t="n">
+      <c r="L36" s="33" t="n">
         <v>1571.63023196731</v>
       </c>
       <c r="M36" s="9" t="n">
@@ -79665,7 +79615,7 @@
         <v>103</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q36" s="6" t="n">
         <v>75</v>
@@ -79738,7 +79688,7 @@
       <c r="K37" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L37" s="34" t="n">
+      <c r="L37" s="33" t="n">
         <v>1472.57040072013</v>
       </c>
       <c r="M37" s="9" t="n">
@@ -79748,7 +79698,7 @@
         <v>103</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q37" s="6" t="n">
         <v>75</v>
@@ -79821,7 +79771,7 @@
       <c r="K38" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L38" s="34" t="n">
+      <c r="L38" s="33" t="n">
         <v>1374.26861868423</v>
       </c>
       <c r="M38" s="9" t="n">
@@ -79831,7 +79781,7 @@
         <v>103</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q38" s="6" t="n">
         <v>75</v>
@@ -79904,7 +79854,7 @@
       <c r="K39" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L39" s="34" t="n">
+      <c r="L39" s="33" t="n">
         <v>1274.84417585507</v>
       </c>
       <c r="M39" s="9" t="n">
@@ -79914,7 +79864,7 @@
         <v>103</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q39" s="6" t="n">
         <v>75</v>
@@ -79955,7 +79905,7 @@
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0.75</v>
@@ -79987,7 +79937,7 @@
       <c r="K40" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L40" s="34" t="n">
+      <c r="L40" s="33" t="n">
         <v>1673.93334014304</v>
       </c>
       <c r="M40" s="9" t="n">
@@ -79997,7 +79947,7 @@
         <v>103</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q40" s="6" t="n">
         <v>75</v>
@@ -80038,7 +79988,7 @@
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0.75</v>
@@ -80070,7 +80020,7 @@
       <c r="K41" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L41" s="34" t="n">
+      <c r="L41" s="33" t="n">
         <v>1572.61981524537</v>
       </c>
       <c r="M41" s="9" t="n">
@@ -80080,7 +80030,7 @@
         <v>103</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q41" s="6" t="n">
         <v>75</v>
@@ -80121,7 +80071,7 @@
     </row>
     <row r="42" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0.75</v>
@@ -80153,7 +80103,7 @@
       <c r="K42" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L42" s="34" t="n">
+      <c r="L42" s="33" t="n">
         <v>1472.36614172608</v>
       </c>
       <c r="M42" s="9" t="n">
@@ -80163,7 +80113,7 @@
         <v>103</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q42" s="6" t="n">
         <v>75</v>
@@ -80204,7 +80154,7 @@
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0.75</v>
@@ -80236,7 +80186,7 @@
       <c r="K43" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L43" s="34" t="n">
+      <c r="L43" s="33" t="n">
         <v>1374.04625068217</v>
       </c>
       <c r="M43" s="9" t="n">
@@ -80246,7 +80196,7 @@
         <v>103</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q43" s="6" t="n">
         <v>75</v>
@@ -80287,7 +80237,7 @@
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0.75</v>
@@ -80319,7 +80269,7 @@
       <c r="K44" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L44" s="34" t="n">
+      <c r="L44" s="33" t="n">
         <v>1275.38376886076</v>
       </c>
       <c r="M44" s="9" t="n">
@@ -80329,7 +80279,7 @@
         <v>103</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q44" s="6" t="n">
         <v>75</v>
@@ -80563,10 +80513,10 @@
         <v>10</v>
       </c>
       <c r="B58" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>433</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>434</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>435.8</v>
@@ -80683,7 +80633,7 @@
         <v>19</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K63" s="0" t="n">
         <v>15</v>
@@ -80701,15 +80651,15 @@
         <v>15</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K64" s="0" t="n">
         <v>1</v>
       </c>
       <c r="N64" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="O64" s="35" t="n">
+        <v>436</v>
+      </c>
+      <c r="O64" s="34" t="n">
         <v>0.9</v>
       </c>
     </row>
@@ -80725,15 +80675,15 @@
         <v>15</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K65" s="0" t="n">
         <v>20</v>
       </c>
       <c r="N65" s="0" t="s">
-        <v>439</v>
-      </c>
-      <c r="O65" s="35" t="n">
+        <v>438</v>
+      </c>
+      <c r="O65" s="34" t="n">
         <v>0.198</v>
       </c>
     </row>
@@ -80749,20 +80699,20 @@
         <v>6</v>
       </c>
       <c r="N66" s="0" t="s">
-        <v>440</v>
-      </c>
-      <c r="O66" s="35" t="n">
+        <v>439</v>
+      </c>
+      <c r="O66" s="34" t="n">
         <v>0.98</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I67" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="N67" s="0" t="s">
         <v>441</v>
       </c>
-      <c r="N67" s="0" t="s">
-        <v>442</v>
-      </c>
-      <c r="O67" s="35" t="n">
+      <c r="O67" s="34" t="n">
         <v>0.006</v>
       </c>
       <c r="Q67" s="0" t="n">
@@ -80807,9 +80757,9 @@
         <v>0.181940721899832</v>
       </c>
       <c r="N68" s="0" t="s">
-        <v>443</v>
-      </c>
-      <c r="O68" s="35" t="n">
+        <v>442</v>
+      </c>
+      <c r="O68" s="34" t="n">
         <v>0.02</v>
       </c>
     </row>
@@ -80841,9 +80791,9 @@
         <v>0.180401166165974</v>
       </c>
       <c r="N69" s="0" t="s">
-        <v>444</v>
-      </c>
-      <c r="O69" s="35" t="n">
+        <v>443</v>
+      </c>
+      <c r="O69" s="34" t="n">
         <v>100</v>
       </c>
       <c r="Q69" s="0" t="n">

</xml_diff>